<commit_message>
Catalogue : début du scan du catalogue Winter 18
</commit_message>
<xml_diff>
--- a/Catalogues/catalogoModeleFormat.EAN13.xlsx
+++ b/Catalogues/catalogoModeleFormat.EAN13.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m312742\Documents\Perso\obg\Catalogues2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m312742\Documents\Perso\obg\Catalogues\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="catalogo Modèle format.EAN13" sheetId="1" r:id="rId1"/>
@@ -553,11 +553,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -603,7 +604,65 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -894,17 +953,18 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -927,7 +987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>8050846049154</v>
       </c>
@@ -937,7 +997,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
@@ -950,7 +1010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -960,7 +1020,7 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
@@ -975,8 +1035,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:G50000">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>LEFT($B2,15)&lt;&gt;LEFT($B1,15)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:E50000">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>LEFT($C2,4)&lt;&gt;LEFT($C1,4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A50000">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(LEFT($A1,1) &lt;&gt; "8",LEFT($A1,1) &lt;&gt; "3", LEFT($A1,1) &lt;&gt; "C")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Catalogue : scan Spring 19
</commit_message>
<xml_diff>
--- a/Catalogues/catalogoModeleFormat.EAN13.xlsx
+++ b/Catalogues/catalogoModeleFormat.EAN13.xlsx
@@ -553,12 +553,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -604,18 +605,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -631,35 +621,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -962,6 +923,7 @@
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="4"/>
+    <col min="5" max="5" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1000,7 +962,7 @@
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
@@ -1023,7 +985,7 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
@@ -1035,17 +997,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:G50000">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>LEFT($B2,15)&lt;&gt;LEFT($B1,15)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E50000">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>LEFT($C2,4)&lt;&gt;LEFT($C1,4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A50000">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(LEFT($A1,1) &lt;&gt; "8",LEFT($A1,1) &lt;&gt; "3", LEFT($A1,1) &lt;&gt; "C")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>